<commit_message>
Added some new bugs.
</commit_message>
<xml_diff>
--- a/COMP2160 Assignment 2/Assets/Documentation/Bug History.xlsx
+++ b/COMP2160 Assignment 2/Assets/Documentation/Bug History.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Documents\GitHub\comp2160-ass2-comp2160-assignment-2-group-aw\COMP2160 Assignment 2\Assets\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC8838F-BA30-43AD-8135-5CC2C1EEAD19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD9A65E-0AC9-4841-9ADC-14A421DB22CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{B48CD1F3-4FC5-45D4-9E61-8CB12666AC10}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Bug ID</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Screenshot</t>
   </si>
   <si>
-    <t>Checkpoint.cs/CheckpointManager.cs</t>
-  </si>
-  <si>
     <t>The first checkpoint would not load its glow material when the game first starts, but would on subsequent plays</t>
   </si>
   <si>
@@ -69,10 +66,55 @@
     <t>The first checkpoint will appear to glow a bright green.</t>
   </si>
   <si>
-    <t>The checkpoint will appear its normal colour and look identical to all the others.</t>
-  </si>
-  <si>
     <t>Bug_1.jpg</t>
+  </si>
+  <si>
+    <t>Checkpoint.cs and CheckpointManager.cs</t>
+  </si>
+  <si>
+    <t>CheckpointManager.cs and MenuHandler.cs</t>
+  </si>
+  <si>
+    <t>The checkpoint will appear its normal colour and look identical to all the others due to some sort of race condition</t>
+  </si>
+  <si>
+    <t>If the game ended by the player dying and not hitting every checkpoint, the checkpoint display would overflow with nonsensical entries</t>
+  </si>
+  <si>
+    <t>Reduce the player's health to 0 and do not hit every checkpoint</t>
+  </si>
+  <si>
+    <t>The GameOver screen will display and the checkpoints that were hit will display correctly.</t>
+  </si>
+  <si>
+    <t>The display overflows offscreen and eventually triggers mesh errors in the console</t>
+  </si>
+  <si>
+    <t>Health.cs</t>
+  </si>
+  <si>
+    <t>Reduce the player's health to 0 by running into trees to try and trigger the smoke and explosion effect</t>
+  </si>
+  <si>
+    <t>The smoke effect appears at 50 hp, and the explosion triggers on death</t>
+  </si>
+  <si>
+    <t>Neither particle effect appears</t>
+  </si>
+  <si>
+    <t>The particle effects would not play whatsoever if the particle systems are not acquired by GetComponent</t>
+  </si>
+  <si>
+    <t>The particle effects play even when they should not be triggered</t>
+  </si>
+  <si>
+    <t>Press the play button</t>
+  </si>
+  <si>
+    <t>The smoke or explosion effects will play at 50 hp and 0 hp respectively</t>
+  </si>
+  <si>
+    <t>The smoke and explosions effects play as soon as the game begins, and the smoke repeats.</t>
   </si>
 </sst>
 </file>
@@ -425,16 +467,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD4CAF9E-F279-45DE-8E97-EBB3E8F2B3DE}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" customWidth="1"/>
     <col min="5" max="5" width="45.85546875" customWidth="1"/>
     <col min="7" max="9" width="18.42578125" customWidth="1"/>
     <col min="10" max="10" width="18.28515625" customWidth="1"/>
@@ -483,25 +525,112 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44134</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44139</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
         <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44140</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fleshed out QA Plan, added a number of bugs found during testing.
</commit_message>
<xml_diff>
--- a/COMP2160 Assignment 2/Assets/Documentation/Bug History.xlsx
+++ b/COMP2160 Assignment 2/Assets/Documentation/Bug History.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Documents\GitHub\comp2160-ass2-comp2160-assignment-2-group-aw\COMP2160 Assignment 2\Assets\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\GitHub\comp2160-ass2-comp2160-assignment-2-group-aw\COMP2160 Assignment 2\Assets\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD9A65E-0AC9-4841-9ADC-14A421DB22CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6BA770-0FB4-4F95-902E-763A2035E9E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{B48CD1F3-4FC5-45D4-9E61-8CB12666AC10}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B48CD1F3-4FC5-45D4-9E61-8CB12666AC10}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>Bug ID</t>
   </si>
@@ -69,12 +69,6 @@
     <t>Bug_1.jpg</t>
   </si>
   <si>
-    <t>Checkpoint.cs and CheckpointManager.cs</t>
-  </si>
-  <si>
-    <t>CheckpointManager.cs and MenuHandler.cs</t>
-  </si>
-  <si>
     <t>The checkpoint will appear its normal colour and look identical to all the others due to some sort of race condition</t>
   </si>
   <si>
@@ -90,9 +84,6 @@
     <t>The display overflows offscreen and eventually triggers mesh errors in the console</t>
   </si>
   <si>
-    <t>Health.cs</t>
-  </si>
-  <si>
     <t>Reduce the player's health to 0 by running into trees to try and trigger the smoke and explosion effect</t>
   </si>
   <si>
@@ -115,6 +106,45 @@
   </si>
   <si>
     <t>The smoke and explosions effects play as soon as the game begins, and the smoke repeats.</t>
+  </si>
+  <si>
+    <t>Car Movement (Drive.cs)</t>
+  </si>
+  <si>
+    <t>Player Health (Health.cs)</t>
+  </si>
+  <si>
+    <t>Checkpoints (Checkpoint.cs and CheckpointManager.cs)</t>
+  </si>
+  <si>
+    <t>The car will not turn in a fixed radius</t>
+  </si>
+  <si>
+    <t>Drive the car and hold down A or D to turn left or right, and keep going until the car has completed a circle.</t>
+  </si>
+  <si>
+    <t>The car completes a turning circle, maintaining the same radius</t>
+  </si>
+  <si>
+    <t>The car seems to slip slightly as it turns, offshooting the fixed radius of the turning circle</t>
+  </si>
+  <si>
+    <t>Camera (SmoothCamAlt.cs)</t>
+  </si>
+  <si>
+    <t>When the car reverses, either by player movement or going backwards down hill, the camera flips around to the other side of the player</t>
+  </si>
+  <si>
+    <t>Drive the car straight up a hill, and then let it slide back downwards, or hold down the S key.</t>
+  </si>
+  <si>
+    <t>The camera remains behind the car, and the car moves backwards towards the bottom of the screen</t>
+  </si>
+  <si>
+    <t>The camera flips around to the other side and shows what is behind the player, similar to a reversing camera</t>
+  </si>
+  <si>
+    <t>Note: While this does function as a reversing camera, and is a somewhat useful side benefit, it is not a one-to-one replication of the camera as seen in the example game</t>
   </si>
 </sst>
 </file>
@@ -150,9 +180,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,170 +505,235 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD4CAF9E-F279-45DE-8E97-EBB3E8F2B3DE}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.42578125" customWidth="1"/>
-    <col min="5" max="5" width="45.85546875" customWidth="1"/>
-    <col min="7" max="9" width="18.42578125" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.44140625" customWidth="1"/>
+    <col min="5" max="5" width="45.88671875" customWidth="1"/>
+    <col min="7" max="9" width="18.44140625" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="3">
         <v>44132</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2">
+        <v>3.1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>44134</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>44139</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
-        <v>13</v>
-      </c>
+      <c r="H4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>44134</v>
-      </c>
-      <c r="C3">
+    <row r="5" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>44140</v>
+      </c>
+      <c r="C5" s="2">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>44142</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" t="s">
-        <v>29</v>
-      </c>
+      <c r="E6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="7" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44142</v>
+      </c>
+      <c r="C7" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
-        <v>44139</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>44140</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" t="s">
-        <v>24</v>
+      <c r="D7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="2">
+        <v>5.2</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the way Checkpoints are handled by the GameOverMenu to match the specification; added it to bug history
</commit_message>
<xml_diff>
--- a/COMP2160 Assignment 2/Assets/Documentation/Bug History.xlsx
+++ b/COMP2160 Assignment 2/Assets/Documentation/Bug History.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\GitHub\comp2160-ass2-comp2160-assignment-2-group-aw\COMP2160 Assignment 2\Assets\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Documents\GitHub\comp2160-ass2-comp2160-assignment-2-group-aw\COMP2160 Assignment 2\Assets\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6BA770-0FB4-4F95-902E-763A2035E9E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D186EBF-F7F1-427A-AB9B-15E3E9FC6D6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B48CD1F3-4FC5-45D4-9E61-8CB12666AC10}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{B48CD1F3-4FC5-45D4-9E61-8CB12666AC10}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>Bug ID</t>
   </si>
@@ -145,6 +145,18 @@
   </si>
   <si>
     <t>Note: While this does function as a reversing camera, and is a somewhat useful side benefit, it is not a one-to-one replication of the camera as seen in the example game</t>
+  </si>
+  <si>
+    <t>Game Over Menu would display only the completed checkpoints, rather than marking all untouched ones as "Incomplete" in the menu</t>
+  </si>
+  <si>
+    <t>Drive the car and hit a number of checkpoints, but not all of them. Reduce the car's health to zero to bring up the game over menu</t>
+  </si>
+  <si>
+    <t>The game over menu displays all existing checkpoints in the scene. If they are complete, the timestamp of when they were hit is shown, otherwise they are shown as "Incomplete".</t>
+  </si>
+  <si>
+    <t>The game over menu only displays the checkpoints which were hit</t>
   </si>
 </sst>
 </file>
@@ -180,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -191,6 +203,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,22 +518,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD4CAF9E-F279-45DE-8E97-EBB3E8F2B3DE}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.44140625" customWidth="1"/>
-    <col min="5" max="5" width="45.88671875" customWidth="1"/>
-    <col min="7" max="9" width="18.44140625" customWidth="1"/>
-    <col min="10" max="10" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" customWidth="1"/>
+    <col min="5" max="5" width="45.85546875" customWidth="1"/>
+    <col min="7" max="9" width="18.42578125" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -552,7 +565,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -584,7 +597,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -614,7 +627,7 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -644,7 +657,7 @@
       </c>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -674,7 +687,7 @@
       </c>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -704,7 +717,7 @@
       </c>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -734,6 +747,35 @@
       </c>
       <c r="J7" s="2" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>44143</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>